<commit_message>
Updated code to show remaining 1. Remaining unmatched record in Payments 2. Acc. Errors now shows only errors 3. Columns of all files to be renamed as per Payments format and joined
</commit_message>
<xml_diff>
--- a/Accounts.xlsx
+++ b/Accounts.xlsx
@@ -22,10 +22,10 @@
     <t>TRUCK NO</t>
   </si>
   <si>
-    <t>Accepted Qty</t>
-  </si>
-  <si>
-    <t>Received Qty</t>
+    <t>ACC.</t>
+  </si>
+  <si>
+    <t>REC.</t>
   </si>
   <si>
     <t>PRICE</t>
@@ -40,7 +40,7 @@
     <t>GRAND TOTAL</t>
   </si>
   <si>
-    <t>FRT</t>
+    <t>FRT.</t>
   </si>
   <si>
     <t>T PAID</t>

</xml_diff>